<commit_message>
Updating the data sources page for CSEntry, which necessitated the revision of the excel file and jpg, and the inclusion of the HGI files into the CSPro helps folder (they were pulled from the CSBatch folder)
</commit_message>
<xml_diff>
--- a/CSPro/topics/logic/export/Tables used to create pngs for export hgts.xlsx
+++ b/CSPro/topics/logic/export/Tables used to create pngs for export hgts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\helps\CSPro\topics\logic\export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7C961D-7839-4913-B744-11A5AF003EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48962E8-728B-42CE-A2F3-808A2CD05B52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="803" activeTab="3" xr2:uid="{43B329F7-FB55-4B9E-9ACE-74BC33261969}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="78">
   <si>
     <t>CSPro DB</t>
   </si>
@@ -1291,7 +1291,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1764,10 +1764,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F88AC215-0C21-4EAD-B944-6EFF7FF0D019}">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1784,7 +1784,7 @@
     <col min="10" max="10" width="5.44140625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>71</v>
       </c>
@@ -1814,7 +1814,7 @@
       </c>
       <c r="J1" s="10"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>69</v>
       </c>
@@ -1827,7 +1827,7 @@
       <c r="H2" s="42"/>
       <c r="I2" s="42"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>3</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="H3" s="22"/>
       <c r="I3" s="22"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
@@ -1867,7 +1867,7 @@
       <c r="H4" s="22"/>
       <c r="I4" s="22"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>41</v>
       </c>
@@ -1888,7 +1888,7 @@
       <c r="H5" s="22"/>
       <c r="I5" s="22"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
         <v>46</v>
       </c>
@@ -1909,7 +1909,7 @@
       <c r="H6" s="22"/>
       <c r="I6" s="22"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
@@ -1919,9 +1919,7 @@
       <c r="C7" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="D7" s="19"/>
       <c r="E7" s="21" t="s">
         <v>30</v>
       </c>
@@ -1934,7 +1932,7 @@
       <c r="H7" s="22"/>
       <c r="I7" s="22"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
@@ -1953,7 +1951,7 @@
       <c r="H8" s="22"/>
       <c r="I8" s="22"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="14" t="s">
         <v>9</v>
       </c>
@@ -1963,9 +1961,7 @@
       <c r="C9" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="D9" s="19"/>
       <c r="E9" s="21" t="s">
         <v>30</v>
       </c>
@@ -1974,7 +1970,7 @@
       <c r="H9" s="22"/>
       <c r="I9" s="22"/>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>10</v>
       </c>
@@ -1984,9 +1980,7 @@
       <c r="C10" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="31" t="s">
-        <v>30</v>
-      </c>
+      <c r="D10" s="19"/>
       <c r="E10" s="32" t="s">
         <v>30</v>
       </c>
@@ -1995,7 +1989,7 @@
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
         <v>48</v>
       </c>
@@ -2005,9 +1999,7 @@
       <c r="C11" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="D11" s="19"/>
       <c r="E11" s="21" t="s">
         <v>30</v>
       </c>
@@ -2016,7 +2008,7 @@
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="14" t="s">
         <v>47</v>
       </c>
@@ -2026,9 +2018,7 @@
       <c r="C12" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="D12" s="19"/>
       <c r="E12" s="21" t="s">
         <v>30</v>
       </c>
@@ -2037,7 +2027,7 @@
       <c r="H12" s="22"/>
       <c r="I12" s="22"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="14" t="s">
         <v>68</v>
       </c>
@@ -2056,7 +2046,7 @@
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="14" t="s">
         <v>4</v>
       </c>
@@ -2066,9 +2056,7 @@
       <c r="C14" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="D14" s="19"/>
       <c r="E14" s="20" t="s">
         <v>30</v>
       </c>
@@ -2083,7 +2071,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="42" t="s">
         <v>70</v>
       </c>
@@ -2096,39 +2084,56 @@
       <c r="H15" s="42"/>
       <c r="I15" s="42"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="22"/>
+        <v>20</v>
+      </c>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="19"/>
       <c r="F16" s="19"/>
       <c r="G16" s="19"/>
-      <c r="H16" s="21" t="s">
-        <v>30</v>
-      </c>
+      <c r="H16" s="19"/>
       <c r="I16" s="22"/>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="18" t="s">
-        <v>67</v>
+      <c r="A17" s="14" t="s">
+        <v>33</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="C17" s="22"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="20" t="s">
-        <v>30</v>
-      </c>
+      <c r="E17" s="22"/>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
+      <c r="H17" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="22"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>